<commit_message>
add training and prediction code for stratified data
</commit_message>
<xml_diff>
--- a/eda/data_summary.xlsx
+++ b/eda/data_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naghamdaood/Projects/video-based-seizure-detection-challenge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naghamdaood/Projects/video-based-seizure-detection-challenge/eda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448D306-1E47-684A-BA8E-875AFCCF8D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422467CC-C88C-F144-AB6D-AE5781E81220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4388,6 +4388,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4454,7 +4455,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4762,8 +4763,8 @@
   <dimension ref="A1:F1441"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>